<commit_message>
dev-1.1.0 : # Update Report NG only by month
</commit_message>
<xml_diff>
--- a/storage/template/Export_NG.xlsx
+++ b/storage/template/Export_NG.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\avicennaa\storage\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\00_Project\avicenna\storage\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,21 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>NO</t>
+    <t>tanggal</t>
   </si>
   <si>
-    <t>JENIS NG</t>
+    <t>Total</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>LINE</t>
-  </si>
-  <si>
-    <t>DATA NG PERIODE</t>
+    <t>Nama NG</t>
   </si>
 </sst>
 </file>
@@ -55,11 +49,10 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -71,12 +64,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -99,11 +92,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -111,11 +167,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,45 +477,1118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:AG165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AG164" sqref="AG164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="21.28515625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="30.90625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="2" customWidth="1"/>
+    <col min="5" max="33" width="9.1796875" style="2"/>
+    <col min="34" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A2" s="9"/>
+      <c r="AG2" s="7"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="AG3" s="2">
+        <f>SUM(B3:AF3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="AG4" s="2">
+        <f t="shared" ref="AG4:AG67" si="0">SUM(B4:AF4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="AG5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="AG6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AG7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AG8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AG9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AG10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AG11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AG12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AG13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AG14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AG15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AG16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG38" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG39" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG40" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG41" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG42" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG43" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG44" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG45" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG46" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG47" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG48" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG49" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG50" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG51" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG52" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG53" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG54" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG55" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG56" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG57" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG58" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG59" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG60" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG61" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG62" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG63" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG64" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG65" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG66" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG67" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG68" s="2">
+        <f t="shared" ref="AG68:AG131" si="1">SUM(B68:AF68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG69" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG70" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG71" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG72" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG73" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG74" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG75" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG76" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG77" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG78" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG79" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG80" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG81" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG82" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG83" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG84" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG85" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG86" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG87" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG88" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG89" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG90" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG91" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG92" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG93" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG94" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG95" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG96" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG97" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG98" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG99" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG100" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG101" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG102" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG103" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG104" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG105" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG106" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG107" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG108" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG109" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG110" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG111" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG112" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG113" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG114" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG115" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG116" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG117" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG118" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG119" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG120" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG121" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG122" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG123" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG124" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG125" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG126" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG127" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG128" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG129" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG130" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG131" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG132" s="2">
+        <f t="shared" ref="AG132:AG165" si="2">SUM(B132:AF132)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG133" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG134" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG135" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG136" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG137" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG138" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG139" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG140" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG141" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG142" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG143" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG144" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG145" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG146" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG147" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG148" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG149" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG150" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG151" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG152" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG153" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG154" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG155" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG156" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG157" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG158" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG159" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG160" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG161" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG162" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG163" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG164" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="33:33" x14ac:dyDescent="0.35">
+      <c r="AG165" s="2">
+        <f>SUM(B165:AF165)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="3">
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>